<commit_message>
code o quan Net
</commit_message>
<xml_diff>
--- a/TasksBugsList.xlsx
+++ b/TasksBugsList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\demWcontest\Wcontest-Team2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCB84E67-A894-4EDA-91EB-55D03EA3752B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{767B0BEA-F099-4472-A2AF-B8BD676FAEF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4D43132C-1E09-488E-BB0E-21797307D290}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="52">
   <si>
     <t>No</t>
   </si>
@@ -198,36 +198,35 @@
  người dùng đăng ký tài khoản, lấy lại mật khẩu</t>
   </si>
   <si>
-    <t>Sử dụng phần mềm Xara Web Designer,
+    <t>24/02/2023</t>
+  </si>
+  <si>
+    <t>Thiết kế (vẽ ra) giao diện cho các phần của trang web</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Hoang + Khoi</t>
+  </si>
+  <si>
+    <t>Trang web khá giống leetcode,
+ bonus thêm phần đấu trường nếu có thể</t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t>Sử dụng figma, 
   tham khảo leetcode,
  các trang web trên mạng</t>
   </si>
   <si>
-    <t>24/02/2023</t>
-  </si>
-  <si>
-    <t>Thiết kế (vẽ ra) giao diện cho các phần của trang web</t>
-  </si>
-  <si>
-    <t>Done</t>
-  </si>
-  <si>
-    <t>Hoang + Khoi</t>
-  </si>
-  <si>
-    <t>Tiếp tục cải thiện, hoàn thiện thì làm task 12</t>
-  </si>
-  <si>
-    <t>Trang web khá giống leetcode,
- bonus thêm phần đấu trường nếu có thể</t>
-  </si>
-  <si>
-    <t>Pending</t>
-  </si>
-  <si>
-    <t>Pending,
- Khôi làm phần đăng nhập, 
-Hoàng làm phần đăng ký</t>
+    <t>Thiết kế database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pending,
+ </t>
   </si>
 </sst>
 </file>
@@ -660,7 +659,7 @@
   <dimension ref="A1:J69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="72" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -874,8 +873,8 @@
       <c r="H7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>48</v>
+      <c r="I7" s="9" t="s">
+        <v>45</v>
       </c>
       <c r="J7" s="5" t="s">
         <v>30</v>
@@ -907,7 +906,7 @@
         <v>38</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J8" s="5" t="s">
         <v>32</v>
@@ -939,7 +938,7 @@
         <v>39</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>34</v>
@@ -971,13 +970,13 @@
         <v>40</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1000,7 +999,7 @@
         <v>45049</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>51</v>
@@ -1038,13 +1037,13 @@
         <v>2</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G13" s="3">
         <v>45049</v>
@@ -1052,26 +1051,44 @@
       <c r="H13" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I13" s="1"/>
+      <c r="I13" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="J13" s="5" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="3"/>
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="3">
+        <v>45080</v>
+      </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>

</xml_diff>